<commit_message>
minor bug fix on community entity
</commit_message>
<xml_diff>
--- a/FE/allocation_results.xlsx
+++ b/FE/allocation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,14 +564,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Barangay Hall Nagbalon</t>
+          <t>Old Municipal Bldg.</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>120.950788291388</v>
+        <v>120.948177254006</v>
       </c>
       <c r="F4" t="n">
-        <v>14.7523618894178</v>
+        <v>14.7573006861396</v>
       </c>
       <c r="G4" t="n">
         <v>5000</v>
@@ -634,14 +634,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Lias Elementary School</t>
+          <t>Ibayo Elementary School</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>120.965390844846</v>
+        <v>120.959816737558</v>
       </c>
       <c r="F6" t="n">
-        <v>14.7627779447143</v>
+        <v>14.7535649557989</v>
       </c>
       <c r="G6" t="n">
         <v>1545</v>
@@ -739,14 +739,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Saog Elementary School</t>
+          <t>FSS Patulo Elementary School</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>120.956198167611</v>
+        <v>121.027062736924</v>
       </c>
       <c r="F9" t="n">
-        <v>14.765465938427</v>
+        <v>14.7839553140957</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -774,14 +774,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Old Municipal Bldg.</t>
+          <t>Barangay Hall Nagbalon</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>120.948177254006</v>
+        <v>120.950788291388</v>
       </c>
       <c r="F10" t="n">
-        <v>14.7573006861396</v>
+        <v>14.7523618894178</v>
       </c>
       <c r="G10" t="n">
         <v>3000</v>
@@ -973,68 +973,33 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Saog</t>
+          <t>Tabing Ilog</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>120.9556</v>
+        <v>120.9488</v>
       </c>
       <c r="C16" t="n">
-        <v>14.7642</v>
+        <v>14.7649</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Saog Elementary School</t>
+          <t>Barangay Hall Tabing Ilog</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>120.956198167611</v>
+        <v>120.948513036352</v>
       </c>
       <c r="F16" t="n">
-        <v>14.765465938427</v>
+        <v>14.7656033896092</v>
       </c>
       <c r="G16" t="n">
-        <v>15000</v>
+        <v>5500</v>
       </c>
       <c r="H16" t="n">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="I16" t="inlineStr">
-        <is>
-          <t>Level 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Tabing Ilog</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>120.9488</v>
-      </c>
-      <c r="C17" t="n">
-        <v>14.7649</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Barangay Hall Tabing Ilog</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>120.948513036352</v>
-      </c>
-      <c r="F17" t="n">
-        <v>14.7656033896092</v>
-      </c>
-      <c r="G17" t="n">
-        <v>5500</v>
-      </c>
-      <c r="H17" t="n">
-        <v>55</v>
-      </c>
-      <c r="I17" t="inlineStr">
         <is>
           <t>Level 1</t>
         </is>

</xml_diff>

<commit_message>
renamed shelterData to shelData
</commit_message>
<xml_diff>
--- a/FE/allocation_results.xlsx
+++ b/FE/allocation_results.xlsx
@@ -634,14 +634,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Lias Elementary School</t>
+          <t>Ibayo Elementary School</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>120.965390844846</v>
+        <v>120.959816737558</v>
       </c>
       <c r="F6" t="n">
-        <v>14.7627779447143</v>
+        <v>14.7535649557989</v>
       </c>
       <c r="G6" t="n">
         <v>1545</v>
@@ -704,14 +704,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Barangay Hall Nagbalon</t>
+          <t>Old Municipal Bldg.</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>120.950788291388</v>
+        <v>120.948177254006</v>
       </c>
       <c r="F8" t="n">
-        <v>14.7523618894178</v>
+        <v>14.7573006861396</v>
       </c>
       <c r="G8" t="n">
         <v>4925</v>
@@ -739,14 +739,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Saog Elementary School</t>
+          <t>Marilao Central School</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>120.956198167611</v>
+        <v>120.949191076043</v>
       </c>
       <c r="F9" t="n">
-        <v>14.765465938427</v>
+        <v>14.7549081782114</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -774,14 +774,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Old Municipal Bldg.</t>
+          <t>Barangay Hall Nagbalon</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>120.948177254006</v>
+        <v>120.950788291388</v>
       </c>
       <c r="F10" t="n">
-        <v>14.7573006861396</v>
+        <v>14.7523618894178</v>
       </c>
       <c r="G10" t="n">
         <v>3000</v>

</xml_diff>

<commit_message>
bugfixes, removed maxdistance func
</commit_message>
<xml_diff>
--- a/FE/allocation_results.xlsx
+++ b/FE/allocation_results.xlsx
@@ -494,14 +494,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Abangan Sur Elementary School</t>
+          <t>Tabing Ilog Elementary School</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>120.942286137427</v>
+        <v>120.948821314155</v>
       </c>
       <c r="F2" t="n">
-        <v>14.7647143396197</v>
+        <v>14.7652274561484</v>
       </c>
       <c r="G2" t="n">
         <v>10080</v>
@@ -634,14 +634,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ibayo Elementary School</t>
+          <t>Lias Elementary School</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>120.959816737558</v>
+        <v>120.965390844846</v>
       </c>
       <c r="F6" t="n">
-        <v>14.7535649557989</v>
+        <v>14.7627779447143</v>
       </c>
       <c r="G6" t="n">
         <v>1545</v>
@@ -704,14 +704,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Old Municipal Bldg.</t>
+          <t>Barangay Hall Nagbalon</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>120.948177254006</v>
+        <v>120.950788291388</v>
       </c>
       <c r="F8" t="n">
-        <v>14.7573006861396</v>
+        <v>14.7523618894178</v>
       </c>
       <c r="G8" t="n">
         <v>4925</v>
@@ -739,14 +739,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Marilao Central School</t>
+          <t>Ramcar Covered Court</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>120.949191076043</v>
+        <v>120.954403339867</v>
       </c>
       <c r="F9" t="n">
-        <v>14.7549081782114</v>
+        <v>14.7646177280722</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -774,14 +774,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Barangay Hall Nagbalon</t>
+          <t>Old Municipal Bldg.</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>120.950788291388</v>
+        <v>120.948177254006</v>
       </c>
       <c r="F10" t="n">
-        <v>14.7523618894178</v>
+        <v>14.7573006861396</v>
       </c>
       <c r="G10" t="n">
         <v>3000</v>
@@ -1019,14 +1019,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Barangay Hall Tabing Ilog</t>
+          <t>Tabing Ilog Elementary School</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>120.948513036352</v>
+        <v>120.948821314155</v>
       </c>
       <c r="F17" t="n">
-        <v>14.7656033896092</v>
+        <v>14.7652274561484</v>
       </c>
       <c r="G17" t="n">
         <v>5500</v>

</xml_diff>